<commit_message>
Update Gale 2016-2017 BR2
</commit_message>
<xml_diff>
--- a/tests/bin/sample_COUNTER_R4_reports/sample_BR2_reports.xlsx
+++ b/tests/bin/sample_COUNTER_R4_reports/sample_BR2_reports.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereiskind\nolcat\tests\bin\sample_COUNTER_R4_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="EBSCO 16-17" sheetId="1" r:id="rId1"/>
     <sheet name="PQ 16-17" sheetId="3" r:id="rId2"/>
-    <sheet name="Gale 16-17" sheetId="15" r:id="rId3"/>
+    <sheet name="Gale 16-17" sheetId="16" r:id="rId3"/>
     <sheet name="EBSCO 17-18" sheetId="4" r:id="rId4"/>
     <sheet name="PQ 17-18" sheetId="6" r:id="rId5"/>
     <sheet name="Gale 17-18" sheetId="12" r:id="rId6"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="107">
   <si>
     <t/>
   </si>
@@ -1208,25 +1208,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1248,61 +1238,46 @@
       <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
+      <c r="I1" s="3">
+        <v>42552</v>
+      </c>
+      <c r="J1" s="3">
+        <v>42583</v>
+      </c>
+      <c r="K1" s="3">
+        <v>42614</v>
+      </c>
+      <c r="L1" s="3">
+        <v>42644</v>
+      </c>
+      <c r="M1" s="3">
+        <v>42675</v>
+      </c>
+      <c r="N1" s="3">
+        <v>42705</v>
+      </c>
+      <c r="O1" s="3">
+        <v>42736</v>
+      </c>
+      <c r="P1" s="3">
+        <v>42767</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>42795</v>
+      </c>
+      <c r="R1" s="3">
+        <v>42826</v>
+      </c>
+      <c r="S1" s="3">
+        <v>42856</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1315,9 +1290,6 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
       <c r="E3" t="s">
         <v>57</v>
       </c>
@@ -1368,9 +1340,6 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
       <c r="E4" t="s">
         <v>57</v>
       </c>
@@ -1421,9 +1390,6 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
       <c r="E5" t="s">
         <v>57</v>
       </c>
@@ -1477,9 +1443,6 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
       <c r="E6" t="s">
         <v>57</v>
       </c>
@@ -1533,9 +1496,6 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
       <c r="E7" t="s">
         <v>51</v>
       </c>
@@ -1583,9 +1543,6 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
       <c r="E8" t="s">
         <v>51</v>
       </c>
@@ -1636,9 +1593,6 @@
       <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
       <c r="E9" t="s">
         <v>51</v>
       </c>
@@ -1689,9 +1643,6 @@
       <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
       <c r="E10" t="s">
         <v>47</v>
       </c>
@@ -1742,9 +1693,6 @@
       <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
@@ -1795,9 +1743,6 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
       <c r="E12" t="s">
         <v>35</v>
       </c>
@@ -1848,9 +1793,6 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
-        <v>0</v>
-      </c>
       <c r="E13" t="s">
         <v>35</v>
       </c>
@@ -1904,9 +1846,6 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
-        <v>0</v>
-      </c>
       <c r="E14" t="s">
         <v>35</v>
       </c>
@@ -1960,9 +1899,6 @@
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
@@ -2002,6 +1938,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2599,7 +2536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
@@ -3522,7 +3459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add another data source with IR to `bin` files
</commit_message>
<xml_diff>
--- a/tests/bin/sample_COUNTER_R4_reports/sample_BR2_reports.xlsx
+++ b/tests/bin/sample_COUNTER_R4_reports/sample_BR2_reports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="EBSCO 16-17" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="EBSCO 18-19" sheetId="7" r:id="rId7"/>
     <sheet name="PQ 18-19" sheetId="9" r:id="rId8"/>
     <sheet name="Gale 18-19" sheetId="14" r:id="rId9"/>
+    <sheet name="Duke 18-19" sheetId="17" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EBSCO 16-17'!$A$8:$T$8</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="114">
   <si>
     <t/>
   </si>
@@ -358,13 +359,34 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2019-09-05</t>
+  </si>
+  <si>
+    <t>Silverchair</t>
+  </si>
+  <si>
+    <t>SoundAn Acoulogical Treatise</t>
+  </si>
+  <si>
+    <t>Duke University Press</t>
+  </si>
+  <si>
+    <t>10.1215/9780822374824</t>
+  </si>
+  <si>
+    <t>978-0-8223-6022-3</t>
+  </si>
+  <si>
+    <t>978-0-8223-7482-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,13 +401,43 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF578FAE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCD2DE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -397,10 +449,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -410,9 +463,26 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1036,6 +1106,270 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="36" style="6" customWidth="1"/>
+    <col min="3" max="10" width="10.7109375" style="6" customWidth="1"/>
+    <col min="11" max="20" width="5.42578125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="224.5703125" style="6" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="9">
+        <v>2</v>
+      </c>
+      <c r="S9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
+        <v>2</v>
+      </c>
+      <c r="S10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" useFirstPageNumber="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
@@ -3459,7 +3793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>